<commit_message>
initial Miiw store online, asp.net MVC+EF (code first)
</commit_message>
<xml_diff>
--- a/Docs/DBSchema.xlsx
+++ b/Docs/DBSchema.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\MiiwStore\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\miiwstore\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Product" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="Order" sheetId="5" r:id="rId5"/>
     <sheet name="OrderDetail" sheetId="8" r:id="rId6"/>
     <sheet name="User" sheetId="7" r:id="rId7"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="37">
   <si>
     <t>field name</t>
   </si>
@@ -139,6 +138,9 @@
   </si>
   <si>
     <t>Amount</t>
+  </si>
+  <si>
+    <t>ProdDetailDesc</t>
   </si>
 </sst>
 </file>
@@ -459,7 +461,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -508,15 +510,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -557,7 +559,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -565,17 +567,25 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -691,7 +701,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:C6"/>
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -758,10 +768,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -799,17 +809,28 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
         <v>35</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -822,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -920,33 +941,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
redesign database, edit product controller
</commit_message>
<xml_diff>
--- a/Docs/DBSchema.xlsx
+++ b/Docs/DBSchema.xlsx
@@ -9,16 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="7"/>
   </bookViews>
   <sheets>
-    <sheet name="Product" sheetId="1" r:id="rId1"/>
-    <sheet name="ProductDetail" sheetId="2" r:id="rId2"/>
-    <sheet name="Category" sheetId="3" r:id="rId3"/>
-    <sheet name="CategoryProduct" sheetId="4" r:id="rId4"/>
-    <sheet name="Order" sheetId="5" r:id="rId5"/>
-    <sheet name="OrderDetail" sheetId="8" r:id="rId6"/>
-    <sheet name="User" sheetId="7" r:id="rId7"/>
+    <sheet name="ProductSet" sheetId="1" r:id="rId1"/>
+    <sheet name="ProductSetDetail" sheetId="9" r:id="rId2"/>
+    <sheet name="Product" sheetId="2" r:id="rId3"/>
+    <sheet name="Category" sheetId="3" r:id="rId4"/>
+    <sheet name="SubCategory" sheetId="10" r:id="rId5"/>
+    <sheet name="User" sheetId="7" r:id="rId6"/>
+    <sheet name="Order" sheetId="5" r:id="rId7"/>
+    <sheet name="OrderDetail" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="41">
   <si>
     <t>field name</t>
   </si>
@@ -44,33 +45,21 @@
     <t>int</t>
   </si>
   <si>
-    <t>ProdName</t>
-  </si>
-  <si>
     <t>string</t>
   </si>
   <si>
     <t>Price</t>
   </si>
   <si>
-    <t>ProdId</t>
-  </si>
-  <si>
     <t>decimal</t>
   </si>
   <si>
-    <t>ProdDetailId</t>
-  </si>
-  <si>
     <t>Field name</t>
   </si>
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>ProdDetalId</t>
-  </si>
-  <si>
     <t>PK</t>
   </si>
   <si>
@@ -80,33 +69,18 @@
     <t>FK</t>
   </si>
   <si>
-    <t>PicURL</t>
-  </si>
-  <si>
-    <t>CatId</t>
-  </si>
-  <si>
-    <t>CatName</t>
-  </si>
-  <si>
     <t>datetime</t>
   </si>
   <si>
     <t>Quantity</t>
   </si>
   <si>
-    <t>OrderId</t>
-  </si>
-  <si>
     <t>BirthDate</t>
   </si>
   <si>
     <t>Address</t>
   </si>
   <si>
-    <t>UserId</t>
-  </si>
-  <si>
     <t>UserName</t>
   </si>
   <si>
@@ -128,9 +102,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>OrderDetailId</t>
-  </si>
-  <si>
     <t>OrderDate</t>
   </si>
   <si>
@@ -140,7 +111,50 @@
     <t>Amount</t>
   </si>
   <si>
-    <t>ProdDetailDesc</t>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>CategoryID</t>
+  </si>
+  <si>
+    <t>Discount</t>
+  </si>
+  <si>
+    <t>ProductSetID</t>
+  </si>
+  <si>
+    <t>ProductID</t>
+  </si>
+  <si>
+    <t>SubCategoryID</t>
+  </si>
+  <si>
+    <t>UserID</t>
+  </si>
+  <si>
+    <t>OrderID</t>
+  </si>
+  <si>
+    <t>RefID</t>
+  </si>
+  <si>
+    <t>enum</t>
+  </si>
+  <si>
+    <t>ProductType</t>
+  </si>
+  <si>
+    <t>P=product
+PS=product set</t>
+  </si>
+  <si>
+    <t>Size</t>
   </si>
 </sst>
 </file>
@@ -176,8 +190,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,21 +478,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -486,10 +506,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -497,10 +517,45 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -510,10 +565,65 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -523,121 +633,94 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
         <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -650,45 +733,45 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C3" sqref="A2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -698,10 +781,176 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -711,24 +960,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -736,10 +985,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -747,18 +996,18 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -766,39 +1015,40 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -806,10 +1056,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -817,10 +1067,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -828,114 +1078,21 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>